<commit_message>
Add new Client in the excel list
</commit_message>
<xml_diff>
--- a/3_DataLayer/rpa_project.xlsx
+++ b/3_DataLayer/rpa_project.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ANUL III\RPA\rpa_project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ANUL III\RPA\rpa_project\3_DataLayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0B3F06-7C0A-4B8F-9DB7-2891F55770C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0FD55BF-3B9A-4A67-AAC8-5CF92D9143BC}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39F59FE-240C-4AFB-BA35-360071DCD783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{A0FD55BF-3B9A-4A67-AAC8-5CF92D9143BC}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Foaie1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -30,101 +31,131 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Galatan Tudor</t>
-  </si>
-  <si>
-    <t>galatan.tudor1@gmail.com</t>
-  </si>
-  <si>
-    <t>Parnau Patrick</t>
-  </si>
-  <si>
-    <t>Dragos Marinescu</t>
-  </si>
-  <si>
-    <t>marinescudragos2014@gmail.com</t>
-  </si>
-  <si>
-    <t>parnaumark17@gmail.com</t>
-  </si>
-  <si>
-    <t>Nume</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <x:si>
+    <x:t>Nume</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Parnau Patrick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>parnaumark17@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dragos Marinescu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marinescudragos2014@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Galatan Tudor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>galatan.tudor1@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dan Petri</x:t>
+  </x:si>
+  <x:si>
+    <x:t>danpetri8@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iris Mihoc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>iris.dm04@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Patrick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>parnau.patrick@yahoo.com</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-  </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Aptos Narrow"/>
+      <x:family val="2"/>
+      <x:charset val="238"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color theme="10"/>
+      <x:name val="Aptos Narrow"/>
+      <x:family val="2"/>
+      <x:charset val="238"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  </x:cellXfs>
+  <x:cellStyles count="2">
+    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,56 +474,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04D1A62-1D83-4DD7-AC5D-AD2ADC705185}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="galatan.tudor1@gmail.com" xr:uid="{4D6B0D86-1179-4BA7-8CD4-3C89AFBFB669}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{97173D32-ED3C-4DFA-9074-DD2FC90AC4BD}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{F92574DC-E834-419C-AEFF-E34BD5860C5A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{E04D1A62-1D83-4DD7-AC5D-AD2ADC705185}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B6"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="O18" sqref="O18"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="14.855469" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:15">
+      <x:c r="A7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="B1" r:id="rId6"/>
+    <x:hyperlink ref="B3" r:id="rId7"/>
+    <x:hyperlink ref="B2" r:id="rId8"/>
+    <x:hyperlink ref="B5" r:id="rId9"/>
+    <x:hyperlink ref="B6" r:id="rId10"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
validare nume si email
</commit_message>
<xml_diff>
--- a/3_DataLayer/rpa_project.xlsx
+++ b/3_DataLayer/rpa_project.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ANUL III\RPA\rpa_project\3_DataLayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39F59FE-240C-4AFB-BA35-360071DCD783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{A0FD55BF-3B9A-4A67-AAC8-5CF92D9143BC}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Foaie1" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="191029"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D616DC5-1B53-4D9F-86E1-53EFC8622CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0FD55BF-3B9A-4A67-AAC8-5CF92D9143BC}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -31,131 +30,119 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <x:si>
-    <x:t>Nume</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Email</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Parnau Patrick</x:t>
-  </x:si>
-  <x:si>
-    <x:t>parnaumark17@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dragos Marinescu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>marinescudragos2014@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Galatan Tudor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>galatan.tudor1@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dan Petri</x:t>
-  </x:si>
-  <x:si>
-    <x:t>danpetri8@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Iris Mihoc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>iris.dm04@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patrick</x:t>
-  </x:si>
-  <x:si>
-    <x:t>parnau.patrick@yahoo.com</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Nume</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Parnau Patrick</t>
+  </si>
+  <si>
+    <t>parnaumark17@gmail.com</t>
+  </si>
+  <si>
+    <t>Dragos Marinescu</t>
+  </si>
+  <si>
+    <t>marinescudragos2014@gmail.com</t>
+  </si>
+  <si>
+    <t>Galatan Tudor</t>
+  </si>
+  <si>
+    <t>galatan.tudor1@gmail.com</t>
+  </si>
+  <si>
+    <t>Dan Petri</t>
+  </si>
+  <si>
+    <t>danpetri8@gmail.com</t>
+  </si>
+  <si>
+    <t>Iris Mihoc</t>
+  </si>
+  <si>
+    <t>iris.dm04@gmail.com</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>parnau.patrick@yahoo.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="3" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Aptos Narrow"/>
-      <x:family val="2"/>
-      <x:charset val="238"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:u/>
-      <x:sz val="11"/>
-      <x:color theme="10"/>
-      <x:name val="Aptos Narrow"/>
-      <x:family val="2"/>
-      <x:charset val="238"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-  </x:cellXfs>
-  <x:cellStyles count="2">
-    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  </cellXfs>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,89 +461,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{E04D1A62-1D83-4DD7-AC5D-AD2ADC705185}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:B6"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="O18" sqref="O18"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="14.855469" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B3" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B5" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B6" s="1" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:15">
-      <x:c r="A7" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:hyperlinks>
-    <x:hyperlink ref="B1" r:id="rId6"/>
-    <x:hyperlink ref="B3" r:id="rId7"/>
-    <x:hyperlink ref="B2" r:id="rId8"/>
-    <x:hyperlink ref="B5" r:id="rId9"/>
-    <x:hyperlink ref="B6" r:id="rId10"/>
-  </x:hyperlinks>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04D1A62-1D83-4DD7-AC5D-AD2ADC705185}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>